<commit_message>
update procesflow RekeningOpenen SaldoInzien GeldOvermaken
</commit_message>
<xml_diff>
--- a/Procesflow/Procesflow_bankzaken.xlsx
+++ b/Procesflow/Procesflow_bankzaken.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mariska Lokhorst\webProject\team-3\Procesflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5AD475-DC07-45B9-9B50-970D8D61ADF1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3CA449-ECB8-4F81-B2F3-1B2BFD6C9769}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{756094F8-9BC3-463D-8EF9-3B55D5B43748}"/>
   </bookViews>
@@ -28,17 +28,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Note: direct na inloggen, zie je al overzicht van rekeningen (incl. saldo)</t>
-  </si>
-  <si>
-    <t>verder kan in dit Overview-scherm worden aangegeven wat verder moet worden gedaan</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -220,7 +209,7 @@
           <a:p>
             <a:r>
               <a:rPr lang="nl-NL" sz="1100"/>
-              <a:t>Persoon</a:t>
+              <a:t>Person</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -282,7 +271,22 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Start pagina van de Vrekbank</a:t>
+            <a:t>Homepage</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t> of the </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>V</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>rekbank</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -293,7 +297,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>knop:</a:t>
+            <a:t>Button:</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
@@ -368,18 +372,15 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Invullen</a:t>
-          </a:r>
+            <a:t>Fill-in information</a:t>
+          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t> gegevens</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>(+ automatisch krijgen van rekeningnummer)</a:t>
+            <a:t>(+ new customer is automatically given an account)</a:t>
           </a:r>
           <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
@@ -506,7 +507,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Klik op knop : wordt lid</a:t>
+            <a:t>"wordt lid"</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -567,7 +568,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Check ingevulde</a:t>
+            <a:t>Check information</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
@@ -708,70 +709,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>260350</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>146050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>412750</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="Tekstballon: ovaal 18">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{066A5F46-16EC-4A74-AA29-2341AAC4445D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6356350" y="3276600"/>
-          <a:ext cx="1371600" cy="692150"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeEllipseCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -89814"/>
-            <a:gd name="adj2" fmla="val 36062"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent4"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent4"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Welke gegevens?</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
@@ -832,7 +769,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Niet ok</a:t>
+            <a:t>Not ok</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1141,7 +1078,7 @@
           <a:p>
             <a:r>
               <a:rPr lang="nl-NL" sz="1100"/>
-              <a:t>Klant</a:t>
+              <a:t>Customer</a:t>
             </a:r>
           </a:p>
         </xdr:txBody>
@@ -1260,7 +1197,18 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Start pagina van de VrekBank</a:t>
+            <a:t>Homepage</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t> of the </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>VrekBank</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1271,7 +1219,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Knop:</a:t>
+            <a:t>Button:</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
@@ -1346,12 +1294,9 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Invullen</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t> login gegevens</a:t>
-          </a:r>
+            <a:t>Fill-in login information</a:t>
+          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100" baseline="0"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -1480,71 +1425,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Klik op knop : login</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>134844</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>50054</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>287244</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>5603</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="39" name="Tekstballon: ovaal 38">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{975A5F67-EA1D-4A9D-AC21-5A567E7A55A9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4422962" y="2291230"/>
-          <a:ext cx="1377576" cy="702608"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeEllipseCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -89814"/>
-            <a:gd name="adj2" fmla="val 36062"/>
-          </a:avLst>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent4"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent4"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Welke gegevens?</a:t>
+            <a:t>"Login"</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1605,11 +1486,11 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Check ingevulde</a:t>
+            <a:t>Check information </a:t>
           </a:r>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t> gegevens (incl db check)</a:t>
+            <a:t>(incl db check)</a:t>
           </a:r>
           <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
@@ -1680,7 +1561,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Niet ok</a:t>
+            <a:t>Not ok</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2005,8 +1886,8 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>119529</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2021,8 +1902,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1917700" y="10185400"/>
-          <a:ext cx="1778000" cy="996950"/>
+          <a:off x="1926665" y="10329209"/>
+          <a:ext cx="1786964" cy="1369732"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2051,42 +1932,48 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Overzicht pagina:</a:t>
+            <a:t>Overview</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t> </a:t>
+            <a:t> page</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>- rekeningen + saldo</a:t>
+            <a:t>- accounts + balance</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>(including business accounts)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>Button:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>- open rekening</a:t>
           </a:r>
           <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
-          <a:endParaRPr lang="nl-NL" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Knop:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>- geld overmaken</a:t>
-          </a:r>
           <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -2096,13 +1983,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
+      <xdr:colOff>369794</xdr:colOff>
       <xdr:row>53</xdr:row>
       <xdr:rowOff>114301</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>587375</xdr:colOff>
+      <xdr:colOff>588869</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>57151</xdr:rowOff>
     </xdr:to>
@@ -2122,8 +2009,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="2760663" y="9920288"/>
-          <a:ext cx="311150" cy="219075"/>
+          <a:off x="2771495" y="10061482"/>
+          <a:ext cx="316380" cy="219075"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -2153,13 +2040,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>107950</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2205,8 +2092,13 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Pagina voor invullen gegevens </a:t>
-          </a:r>
+            <a:t>Page for</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t> transfer information:</a:t>
+          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
@@ -2216,28 +2108,28 @@
           </a:r>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t> debit rekening</a:t>
+            <a:t> debit account</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>- credit naam/rekening</a:t>
+            <a:t>- credit name/account</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>- bedrag</a:t>
+            <a:t>- amount</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>- datum overboeking</a:t>
+            <a:t>- date transfer</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2255,14 +2147,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>383241</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>14942</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>387350</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:colOff>388844</xdr:colOff>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2275,14 +2167,14 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="65" idx="2"/>
+          <a:stCxn id="70" idx="2"/>
           <a:endCxn id="83" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2806700" y="11182350"/>
-          <a:ext cx="19050" cy="1289050"/>
+          <a:off x="2833594" y="13088471"/>
+          <a:ext cx="5603" cy="1052232"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2311,15 +2203,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>251759</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>31376</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:colOff>429559</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>120276</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2334,8 +2226,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2095500" y="11677650"/>
-          <a:ext cx="2006600" cy="273050"/>
+          <a:off x="2089524" y="13478435"/>
+          <a:ext cx="2015564" cy="275665"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2371,13 +2263,8 @@
         <a:p>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Klik op knop:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t> geld overmaken</a:t>
-          </a:r>
-          <a:endParaRPr lang="nl-NL" sz="1100"/>
+            <a:t>"overmaken geld"</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2387,14 +2274,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>463550</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>104588</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>336550</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2409,8 +2296,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1682750" y="14420850"/>
-          <a:ext cx="2311400" cy="660400"/>
+          <a:off x="1688726" y="15979588"/>
+          <a:ext cx="2323353" cy="874059"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -2437,11 +2324,11 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Check db (saldo,</a:t>
+            <a:t>Check db (balance,</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t> naam/rekening combi,...)</a:t>
+            <a:t> name/account combination,...)</a:t>
           </a:r>
           <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
@@ -2452,15 +2339,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>387350</xdr:colOff>
-      <xdr:row>74</xdr:row>
+      <xdr:colOff>388844</xdr:colOff>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>78</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>104588</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2478,8 +2365,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2825750" y="13798550"/>
-          <a:ext cx="12700" cy="622300"/>
+          <a:off x="2839197" y="15486156"/>
+          <a:ext cx="11206" cy="493432"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2509,13 +2396,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>82550</xdr:colOff>
-      <xdr:row>91</xdr:row>
+      <xdr:row>101</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2561,19 +2448,28 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Pagina met secury check</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
+            <a:t>Page</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t> with security check</a:t>
+          </a:r>
           <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>pin?</a:t>
-          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>input of pin </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2583,13 +2479,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:row>103</xdr:row>
       <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>106</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2649,13 +2545,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>520702</xdr:colOff>
-      <xdr:row>99</xdr:row>
+      <xdr:row>109</xdr:row>
       <xdr:rowOff>120653</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>69852</xdr:colOff>
-      <xdr:row>101</xdr:row>
+      <xdr:row>111</xdr:row>
       <xdr:rowOff>25403</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2708,7 +2604,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Niet ok</a:t>
+            <a:t>Not ok</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2719,13 +2615,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>106</xdr:row>
       <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>295277</xdr:colOff>
-      <xdr:row>99</xdr:row>
+      <xdr:row>109</xdr:row>
       <xdr:rowOff>120652</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2777,13 +2673,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>99</xdr:row>
+      <xdr:row>109</xdr:row>
       <xdr:rowOff>139702</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>69850</xdr:colOff>
-      <xdr:row>101</xdr:row>
+      <xdr:row>111</xdr:row>
       <xdr:rowOff>44452</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2847,13 +2743,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>106</xdr:row>
       <xdr:rowOff>152401</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>99</xdr:row>
+      <xdr:row>109</xdr:row>
       <xdr:rowOff>139703</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2903,13 +2799,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>412750</xdr:colOff>
-      <xdr:row>91</xdr:row>
+      <xdr:row>101</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:row>103</xdr:row>
       <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2959,14 +2855,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>103</xdr:row>
+      <xdr:row>113</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>107</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>149412</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2981,8 +2877,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1600200" y="19138900"/>
-          <a:ext cx="2311400" cy="660400"/>
+          <a:off x="1606176" y="20902332"/>
+          <a:ext cx="2323353" cy="911786"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -3009,11 +2905,11 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Geld wordt overgeboekt</a:t>
+            <a:t>Transder of money</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t> (db updaten)</a:t>
+            <a:t> (db update accounts and add transaction)</a:t>
           </a:r>
           <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
@@ -3025,13 +2921,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>101</xdr:row>
+      <xdr:row>111</xdr:row>
       <xdr:rowOff>44452</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>103</xdr:row>
+      <xdr:row>113</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3050,8 +2946,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2733675" y="18643602"/>
-          <a:ext cx="22225" cy="495298"/>
+          <a:off x="2745628" y="20401805"/>
+          <a:ext cx="22225" cy="500527"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3080,15 +2976,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>107950</xdr:colOff>
-      <xdr:row>110</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>117</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>40715</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>98612</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>602503</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>136712</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3103,8 +2999,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1936750" y="20332700"/>
-          <a:ext cx="1778000" cy="1327150"/>
+          <a:off x="1878480" y="20642730"/>
+          <a:ext cx="1786964" cy="1345453"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3133,18 +3029,23 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Pagina met bevestiging</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
+            <a:t>Page</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t> with confirmation of transfer</a:t>
+          </a:r>
           <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Knop:</a:t>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>Button:</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3166,15 +3067,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>88900</xdr:colOff>
+      <xdr:colOff>40714</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>3175</xdr:rowOff>
+      <xdr:rowOff>181723</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>107950</xdr:colOff>
-      <xdr:row>114</xdr:row>
-      <xdr:rowOff>3175</xdr:rowOff>
+      <xdr:colOff>88899</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>24281</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3191,13 +3092,13 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="10800000">
-          <a:off x="1917700" y="10683875"/>
-          <a:ext cx="19050" cy="10312400"/>
+        <a:xfrm rot="10800000" flipH="1">
+          <a:off x="1878479" y="11014076"/>
+          <a:ext cx="48185" cy="12169029"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 5266667"/>
+            <a:gd name="adj1" fmla="val -474422"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -3225,13 +3126,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>167821</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>77</xdr:row>
       <xdr:rowOff>75292</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3472,7 +3373,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Start</a:t>
+            <a:t>Index</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3533,7 +3434,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Start</a:t>
+            <a:t>Index</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3544,13 +3445,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>218515</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>174811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>300691</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>182282</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3605,13 +3506,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>478117</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>44823</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>560293</xdr:colOff>
-      <xdr:row>85</xdr:row>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>52294</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3653,7 +3554,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
-          <a:endParaRPr lang="nl-NL" sz="1100"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>SecurityCheck</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3714,6 +3618,1446 @@
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
             <a:t>Register</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>414244</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Rechte verbindingslijn met pijl 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55E86DAD-C5F3-4F8E-B598-DE1D93CF2D56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="88" idx="4"/>
+          <a:endCxn id="91" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2850403" y="16853647"/>
+          <a:ext cx="14194" cy="319741"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>149412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>321609</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>98612</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Rechte verbindingslijn met pijl 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{912C1DD9-350E-4C55-9F7B-38FB88099B07}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="104" idx="4"/>
+          <a:endCxn id="108" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2767853" y="21814118"/>
+          <a:ext cx="4109" cy="322729"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>102347</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>2989</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>51547</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>14942</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="70" name="Rechthoek 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D37442A7-F266-4ECA-9319-60FBB2B76AA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1940112" y="11955930"/>
+          <a:ext cx="1786964" cy="1132541"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>Account</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t> overview</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>- transaction</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t> history </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>(last 10?)</a:t>
+          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>Button:</a:t>
+          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>- overmaken geld</a:t>
+          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>369794</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>119529</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>383241</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>2989</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Rechte verbindingslijn met pijl 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92F1713A-99CE-4691-B912-A2E02FB38FC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="65" idx="2"/>
+          <a:endCxn id="70" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2820147" y="11698941"/>
+          <a:ext cx="13447" cy="630519"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>194982</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>79188</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>372782</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>168088</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="72" name="Tekstvak 71">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59DB331E-E5B8-456D-9D12-559F180FA4F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2032747" y="11471835"/>
+          <a:ext cx="2015564" cy="275665"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>click on account</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>200212</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>88153</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>282388</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>95623</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="73" name="Rechthoek: afgeronde hoeken 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0812527-D313-4097-AF0C-2CACED87A3C1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3263153" y="11854329"/>
+          <a:ext cx="1307353" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>AccountOverview</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>268940</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>7470</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>97119</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="76" name="Rechthoek: afgeronde hoeken 75">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{912A5A72-0429-47C7-9E55-FBDB61A7D52D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3331881" y="21941118"/>
+          <a:ext cx="1576295" cy="381001"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>ConfirmationTransfer</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>471395</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>5977</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>420594</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>17930</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="77" name="Rechthoek 76">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86579AD1-EEB9-452B-A411-2D27DD3B767C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5372101" y="11958918"/>
+          <a:ext cx="1786964" cy="1132541"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>Application</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t> form</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>Fill in: </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>- name, address, city</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>- BSN</a:t>
+          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>195730</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>173317</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>358588</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>180788</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="79" name="Rechthoek: afgeronde hoeken 78">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2144C25A-48CB-400B-8492-9964AF49E985}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6934201" y="11752729"/>
+          <a:ext cx="1388034" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>AccountApplication</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>203573</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>76573</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>16436</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="81" name="Ovaal 80">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E37E9B9C-B22F-4C47-AAAE-FF1E5E2A40B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5104279" y="13729074"/>
+          <a:ext cx="2323353" cy="668244"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>Check db (BSN)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>139701</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>17930</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>140074</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="84" name="Rechte verbindingslijn met pijl 83">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91A113DE-3141-4E96-AB62-F21676867FFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="77" idx="2"/>
+          <a:endCxn id="81" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6265583" y="13091459"/>
+          <a:ext cx="373" cy="637615"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>179296</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>125137</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>341034</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>29887</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="86" name="Tekstvak 85">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{783EC8A7-44FA-4FC1-86EB-7B454132E19B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8142943" y="14879549"/>
+          <a:ext cx="774326" cy="278279"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>Not ok</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>140075</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>16435</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>566460</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>125136</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="89" name="Verbindingslijn: gebogen 88">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7837E5BA-6B51-4BFA-B549-56C258B10B03}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="81" idx="4"/>
+          <a:endCxn id="86" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="7156916" y="13506358"/>
+          <a:ext cx="482231" cy="2264150"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>179294</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>144186</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>341032</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>48936</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="97" name="Tekstvak 96">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1987D92-3DF6-4413-847B-1BA51E675FED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5692588" y="14898598"/>
+          <a:ext cx="774326" cy="278279"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>Ok</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>566457</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>16437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>140074</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>144187</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="98" name="Verbindingslijn: gebogen 97">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C1E99F1-8942-47E4-814F-D49377F056E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="81" idx="4"/>
+          <a:endCxn id="97" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5922214" y="14554856"/>
+          <a:ext cx="501280" cy="186205"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>303680</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>63874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>252879</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>104589</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="99" name="Rechthoek 98">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF4FE097-D036-4372-AEFB-6A8FD82B33AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5204386" y="15752109"/>
+          <a:ext cx="1786964" cy="1348068"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>Confirmation</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t> page:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>application succeeded</a:t>
+          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>35858</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>117661</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>440765</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>125133</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="101" name="Rechthoek: afgeronde hoeken 100">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35E38AEB-D169-4195-B0EF-02397F9338C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6774329" y="15619132"/>
+          <a:ext cx="1630083" cy="381001"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>Confirmation</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>Application</a:t>
+          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>566457</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>48936</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>584574</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>63874</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="48" name="Rechte verbindingslijn met pijl 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{842854E0-331F-4068-9135-D4286110CB04}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="97" idx="2"/>
+          <a:endCxn id="99" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6079751" y="15176877"/>
+          <a:ext cx="18117" cy="575232"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>46691</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>166967</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>532279</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>59764</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="105" name="Ovaal 104">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDAAE87B-057C-4E9E-8C5A-FB757F553DDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4947397" y="17536085"/>
+          <a:ext cx="2323353" cy="1013385"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>Send email with</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t> confirmation (check db for emailaddress)</a:t>
+          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>584574</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>104589</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>595780</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>166967</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="Rechte verbindingslijn met pijl 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A4DCBBB-6152-460F-870D-AE6A7203F1A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="99" idx="2"/>
+          <a:endCxn id="105" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6097868" y="17100177"/>
+          <a:ext cx="11206" cy="435908"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>181722</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>139701</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>5977</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="116" name="Verbindingslijn: gebogen 115">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{395B160C-3E42-4611-9289-B423A9B4CB94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="65" idx="3"/>
+          <a:endCxn id="77" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3713629" y="11014075"/>
+          <a:ext cx="2551954" cy="1318373"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>257736</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>82177</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>435535</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>171077</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="119" name="Tekstvak 118">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F87F1A1-A499-415A-9A23-9589A7C8C6CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3933265" y="10727765"/>
+          <a:ext cx="2015564" cy="275665"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>"open rekening"</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4020,28 +5364,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77628A9-8BFD-49FE-9150-0DF4141E1CF8}">
-  <dimension ref="J58:J59"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K71" sqref="K71"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I63" sqref="I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="16384" width="8.7265625" style="1"/>
   </cols>
-  <sheetData>
-    <row r="58" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J58" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="10:10" x14ac:dyDescent="0.35">
-      <c r="J59" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
procesflow geupdate rond transfer en open account
</commit_message>
<xml_diff>
--- a/Procesflow/Procesflow_bankzaken.xlsx
+++ b/Procesflow/Procesflow_bankzaken.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mariska Lokhorst\webProject\team-3\Procesflow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Banking\team-3\Procesflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54461FD-E690-4B02-A00D-96C9D8F8BEA5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A86039-110C-4835-ABAD-7495525B66B9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{756094F8-9BC3-463D-8EF9-3B55D5B43748}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{756094F8-9BC3-463D-8EF9-3B55D5B43748}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,11 +23,14 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -115,8 +118,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="520700" y="256615"/>
-          <a:ext cx="920376" cy="1209488"/>
+          <a:off x="520700" y="249144"/>
+          <a:ext cx="896471" cy="1164665"/>
           <a:chOff x="520700" y="254000"/>
           <a:chExt cx="914400" cy="1193800"/>
         </a:xfrm>
@@ -378,10 +381,6 @@
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>(+ new customer is automatically given an account)</a:t>
-          </a:r>
           <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -984,8 +983,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="228600" y="5634691"/>
-          <a:ext cx="917388" cy="1209488"/>
+          <a:off x="228600" y="5410574"/>
+          <a:ext cx="905435" cy="1164664"/>
           <a:chOff x="520700" y="254000"/>
           <a:chExt cx="914400" cy="1193800"/>
         </a:xfrm>
@@ -1302,6 +1301,18 @@
           <a:pPr algn="l"/>
           <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>incl adres</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>, bsn</a:t>
+          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
@@ -2039,15 +2050,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>107950</xdr:colOff>
+      <xdr:colOff>98984</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>84</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>7844</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>143435</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2062,8 +2073,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1936750" y="12471400"/>
-          <a:ext cx="1778000" cy="1327150"/>
+          <a:off x="1900890" y="13813491"/>
+          <a:ext cx="2446992" cy="1874744"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2096,26 +2107,46 @@
           </a:r>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t> transfer information:</a:t>
-          </a:r>
-          <a:endParaRPr lang="nl-NL" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>-</a:t>
-          </a:r>
+            <a:t> transfer </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t> debit account</a:t>
+            <a:t>geeft: </a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>- credit name/account</a:t>
+            <a:t>-debet IBAN (af)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>vraagt: :</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>- credit IBAN</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>- credit lastName</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2129,14 +2160,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>- date transfer</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>- ...</a:t>
+            <a:t>-description </a:t>
           </a:r>
           <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
@@ -2147,15 +2171,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>383241</xdr:colOff>
+      <xdr:colOff>377265</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>14942</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>388844</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>121210</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>7844</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2173,8 +2197,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2833594" y="13088471"/>
-          <a:ext cx="5603" cy="1052232"/>
+          <a:off x="2779806" y="12924118"/>
+          <a:ext cx="344580" cy="889373"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2339,13 +2363,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>388844</xdr:colOff>
-      <xdr:row>84</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:colOff>400051</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>121210</xdr:colOff>
       <xdr:row>87</xdr:row>
       <xdr:rowOff>104588</xdr:rowOff>
     </xdr:to>
@@ -2364,9 +2388,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2839197" y="15486156"/>
-          <a:ext cx="11206" cy="493432"/>
+        <a:xfrm flipH="1">
+          <a:off x="2802592" y="15688235"/>
+          <a:ext cx="321794" cy="14941"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2860,9 +2884,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>118</xdr:row>
-      <xdr:rowOff>149412</xdr:rowOff>
+      <xdr:colOff>412376</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>143435</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2877,8 +2901,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1606176" y="20902332"/>
-          <a:ext cx="2323353" cy="911786"/>
+          <a:off x="1582271" y="20431685"/>
+          <a:ext cx="2433917" cy="1047750"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -2909,7 +2933,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t> (db update accounts and add transaction)</a:t>
+            <a:t> (db update accounts and add transaction, including transaction date</a:t>
           </a:r>
           <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
@@ -2926,7 +2950,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
+      <xdr:colOff>396689</xdr:colOff>
       <xdr:row>113</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
@@ -2946,8 +2970,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2745628" y="20401805"/>
-          <a:ext cx="22225" cy="500527"/>
+          <a:off x="2697816" y="19946099"/>
+          <a:ext cx="101414" cy="485586"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3617,7 +3641,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Register</a:t>
+            <a:t>Registration</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3683,13 +3707,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>118</xdr:row>
-      <xdr:rowOff>149412</xdr:rowOff>
+      <xdr:colOff>321609</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>143435</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>321609</xdr:colOff>
+      <xdr:colOff>396689</xdr:colOff>
       <xdr:row>120</xdr:row>
       <xdr:rowOff>98612</xdr:rowOff>
     </xdr:to>
@@ -3708,9 +3732,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2767853" y="21814118"/>
-          <a:ext cx="4109" cy="322729"/>
+        <a:xfrm flipH="1">
+          <a:off x="2724150" y="21479435"/>
+          <a:ext cx="75080" cy="134471"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3801,6 +3825,13 @@
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
             <a:t>:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>-saldo</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -4172,16 +4203,15 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>- name, address, city</a:t>
+            <a:t>- prive/MKB</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>- BSN</a:t>
-          </a:r>
-          <a:endParaRPr lang="nl-NL" sz="1100"/>
+            <a:t>-indien MKB: sector</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4241,8 +4271,13 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>AccountApplication</a:t>
-          </a:r>
+            <a:t>Open</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>Account</a:t>
+          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4251,15 +4286,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>203573</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>122889</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>158003</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>76573</xdr:colOff>
+      <xdr:colOff>179292</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>16436</xdr:rowOff>
+      <xdr:rowOff>53789</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4274,8 +4309,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5104279" y="13729074"/>
-          <a:ext cx="2323353" cy="668244"/>
+          <a:off x="4927971" y="13425768"/>
+          <a:ext cx="2458945" cy="792256"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -4300,10 +4335,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Check db (BSN)</a:t>
-          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>Create</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t> new account </a:t>
+          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4312,15 +4356,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>139701</xdr:colOff>
+      <xdr:colOff>145677</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>17930</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>140074</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>151091</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>158003</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4338,8 +4382,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6265583" y="13091459"/>
-          <a:ext cx="373" cy="637615"/>
+          <a:off x="6152030" y="12927106"/>
+          <a:ext cx="5414" cy="498662"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4373,10 +4417,10 @@
       <xdr:rowOff>125137</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>341034</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>29887</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>493059</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>71718</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4391,8 +4435,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8142943" y="14879549"/>
-          <a:ext cx="774326" cy="278279"/>
+          <a:off x="7987555" y="14647961"/>
+          <a:ext cx="1515033" cy="484463"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4428,7 +4472,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Not ok</a:t>
+            <a:t>Not ok - is dat een optie?</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4438,13 +4482,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>140075</xdr:colOff>
+      <xdr:colOff>151092</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>16435</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>566460</xdr:colOff>
+      <xdr:rowOff>53788</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>336179</xdr:colOff>
       <xdr:row>81</xdr:row>
       <xdr:rowOff>125136</xdr:rowOff>
     </xdr:to>
@@ -4464,8 +4508,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="7156916" y="13506358"/>
-          <a:ext cx="482231" cy="2264150"/>
+          <a:off x="7236290" y="13139178"/>
+          <a:ext cx="429937" cy="2587628"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -4566,13 +4610,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>566457</xdr:colOff>
+      <xdr:colOff>560481</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>16437</xdr:rowOff>
+      <xdr:rowOff>53790</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>140074</xdr:colOff>
+      <xdr:colOff>151091</xdr:colOff>
       <xdr:row>81</xdr:row>
       <xdr:rowOff>144187</xdr:rowOff>
     </xdr:to>
@@ -4592,8 +4636,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="5922214" y="14554856"/>
-          <a:ext cx="501280" cy="186205"/>
+          <a:off x="5837329" y="14346895"/>
+          <a:ext cx="448986" cy="191245"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -4622,15 +4666,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>303680</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>63874</xdr:rowOff>
+      <xdr:colOff>339539</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>81804</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>252879</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>104589</xdr:rowOff>
+      <xdr:colOff>288738</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>122519</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4645,8 +4689,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5204386" y="15752109"/>
-          <a:ext cx="1786964" cy="1348068"/>
+          <a:off x="5144621" y="15321804"/>
+          <a:ext cx="1751105" cy="1295774"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4686,7 +4730,18 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>application succeeded</a:t>
+            <a:t>application succeeded.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>Vermeldt oa nieuw IBAN</a:t>
           </a:r>
           <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
@@ -4763,15 +4818,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>566457</xdr:colOff>
+      <xdr:colOff>560480</xdr:colOff>
       <xdr:row>83</xdr:row>
       <xdr:rowOff>48936</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>584574</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>63874</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>13820</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>81804</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4788,12 +4843,14 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6079751" y="15176877"/>
-          <a:ext cx="18117" cy="575232"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="5797458" y="15099088"/>
+          <a:ext cx="391456" cy="53975"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="triangle"/>
@@ -4874,7 +4931,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t> confirmation (check db for emailaddress)</a:t>
+            <a:t> confirmation </a:t>
           </a:r>
           <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
@@ -4885,13 +4942,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>584574</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>104589</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>595780</xdr:colOff>
+      <xdr:colOff>589802</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>122519</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>13821</xdr:colOff>
       <xdr:row>95</xdr:row>
       <xdr:rowOff>166967</xdr:rowOff>
     </xdr:to>
@@ -4910,9 +4967,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6097868" y="17100177"/>
-          <a:ext cx="11206" cy="435908"/>
+        <a:xfrm flipH="1">
+          <a:off x="5995520" y="16617578"/>
+          <a:ext cx="24654" cy="582330"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -5366,13 +5423,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77628A9-8BFD-49FE-9150-0DF4141E1CF8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S100" sqref="S100"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O91" sqref="O91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
open account scherm begonnen
</commit_message>
<xml_diff>
--- a/Procesflow/Procesflow_bankzaken.xlsx
+++ b/Procesflow/Procesflow_bankzaken.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Banking\team-3\Procesflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A86039-110C-4835-ABAD-7495525B66B9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25D5EE2-3CDE-49A1-B405-70796806A178}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{756094F8-9BC3-463D-8EF9-3B55D5B43748}"/>
   </bookViews>
@@ -27,10 +27,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5423,8 +5419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77628A9-8BFD-49FE-9150-0DF4141E1CF8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O91" sqref="O91"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updates AccountSummary + Overview Controller
</commit_message>
<xml_diff>
--- a/Procesflow/Procesflow_bankzaken.xlsx
+++ b/Procesflow/Procesflow_bankzaken.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mariska Lokhorst\webProject\team-3\Procesflow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Banking\team-3\Procesflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54461FD-E690-4B02-A00D-96C9D8F8BEA5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25D5EE2-3CDE-49A1-B405-70796806A178}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{756094F8-9BC3-463D-8EF9-3B55D5B43748}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{756094F8-9BC3-463D-8EF9-3B55D5B43748}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -115,8 +114,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="520700" y="256615"/>
-          <a:ext cx="920376" cy="1209488"/>
+          <a:off x="520700" y="249144"/>
+          <a:ext cx="896471" cy="1164665"/>
           <a:chOff x="520700" y="254000"/>
           <a:chExt cx="914400" cy="1193800"/>
         </a:xfrm>
@@ -378,10 +377,6 @@
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>(+ new customer is automatically given an account)</a:t>
-          </a:r>
           <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -984,8 +979,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="228600" y="5634691"/>
-          <a:ext cx="917388" cy="1209488"/>
+          <a:off x="228600" y="5410574"/>
+          <a:ext cx="905435" cy="1164664"/>
           <a:chOff x="520700" y="254000"/>
           <a:chExt cx="914400" cy="1193800"/>
         </a:xfrm>
@@ -1302,6 +1297,18 @@
           <a:pPr algn="l"/>
           <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>incl adres</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>, bsn</a:t>
+          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
+        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
@@ -2039,15 +2046,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>107950</xdr:colOff>
+      <xdr:colOff>98984</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>84</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>7844</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>143435</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2062,8 +2069,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1936750" y="12471400"/>
-          <a:ext cx="1778000" cy="1327150"/>
+          <a:off x="1900890" y="13813491"/>
+          <a:ext cx="2446992" cy="1874744"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2096,26 +2103,46 @@
           </a:r>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t> transfer information:</a:t>
-          </a:r>
-          <a:endParaRPr lang="nl-NL" sz="1100"/>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>-</a:t>
-          </a:r>
+            <a:t> transfer </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t> debit account</a:t>
+            <a:t>geeft: </a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>- credit name/account</a:t>
+            <a:t>-debet IBAN (af)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>vraagt: :</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>- credit IBAN</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>- credit lastName</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2129,14 +2156,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>- date transfer</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>- ...</a:t>
+            <a:t>-description </a:t>
           </a:r>
           <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
@@ -2147,15 +2167,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>383241</xdr:colOff>
+      <xdr:colOff>377265</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>14942</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>388844</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>121210</xdr:colOff>
       <xdr:row>77</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>7844</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2173,8 +2193,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2833594" y="13088471"/>
-          <a:ext cx="5603" cy="1052232"/>
+          <a:off x="2779806" y="12924118"/>
+          <a:ext cx="344580" cy="889373"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2339,13 +2359,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>388844</xdr:colOff>
-      <xdr:row>84</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:colOff>400051</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>121210</xdr:colOff>
       <xdr:row>87</xdr:row>
       <xdr:rowOff>104588</xdr:rowOff>
     </xdr:to>
@@ -2364,9 +2384,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2839197" y="15486156"/>
-          <a:ext cx="11206" cy="493432"/>
+        <a:xfrm flipH="1">
+          <a:off x="2802592" y="15688235"/>
+          <a:ext cx="321794" cy="14941"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2860,9 +2880,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>118</xdr:row>
-      <xdr:rowOff>149412</xdr:rowOff>
+      <xdr:colOff>412376</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>143435</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2877,8 +2897,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1606176" y="20902332"/>
-          <a:ext cx="2323353" cy="911786"/>
+          <a:off x="1582271" y="20431685"/>
+          <a:ext cx="2433917" cy="1047750"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -2909,7 +2929,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t> (db update accounts and add transaction)</a:t>
+            <a:t> (db update accounts and add transaction, including transaction date</a:t>
           </a:r>
           <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
@@ -2926,7 +2946,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
+      <xdr:colOff>396689</xdr:colOff>
       <xdr:row>113</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
@@ -2946,8 +2966,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2745628" y="20401805"/>
-          <a:ext cx="22225" cy="500527"/>
+          <a:off x="2697816" y="19946099"/>
+          <a:ext cx="101414" cy="485586"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3617,7 +3637,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Register</a:t>
+            <a:t>Registration</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -3683,13 +3703,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>118</xdr:row>
-      <xdr:rowOff>149412</xdr:rowOff>
+      <xdr:colOff>321609</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>143435</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>321609</xdr:colOff>
+      <xdr:colOff>396689</xdr:colOff>
       <xdr:row>120</xdr:row>
       <xdr:rowOff>98612</xdr:rowOff>
     </xdr:to>
@@ -3708,9 +3728,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2767853" y="21814118"/>
-          <a:ext cx="4109" cy="322729"/>
+        <a:xfrm flipH="1">
+          <a:off x="2724150" y="21479435"/>
+          <a:ext cx="75080" cy="134471"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3801,6 +3821,13 @@
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
             <a:t>:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>-saldo</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -4172,16 +4199,15 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>- name, address, city</a:t>
+            <a:t>- prive/MKB</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>- BSN</a:t>
-          </a:r>
-          <a:endParaRPr lang="nl-NL" sz="1100"/>
+            <a:t>-indien MKB: sector</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4241,8 +4267,13 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>AccountApplication</a:t>
-          </a:r>
+            <a:t>Open</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>Account</a:t>
+          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4251,15 +4282,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>203573</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>122889</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>158003</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>76573</xdr:colOff>
+      <xdr:colOff>179292</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>16436</xdr:rowOff>
+      <xdr:rowOff>53789</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4274,8 +4305,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5104279" y="13729074"/>
-          <a:ext cx="2323353" cy="668244"/>
+          <a:off x="4927971" y="13425768"/>
+          <a:ext cx="2458945" cy="792256"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -4300,10 +4331,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Check db (BSN)</a:t>
-          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100"/>
+            <a:t>Create</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t> new account </a:t>
+          </a:r>
+          <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4312,15 +4352,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>139701</xdr:colOff>
+      <xdr:colOff>145677</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>17930</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>140074</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>151091</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>158003</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4338,8 +4378,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6265583" y="13091459"/>
-          <a:ext cx="373" cy="637615"/>
+          <a:off x="6152030" y="12927106"/>
+          <a:ext cx="5414" cy="498662"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4373,10 +4413,10 @@
       <xdr:rowOff>125137</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>341034</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>29887</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>493059</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>71718</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4391,8 +4431,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8142943" y="14879549"/>
-          <a:ext cx="774326" cy="278279"/>
+          <a:off x="7987555" y="14647961"/>
+          <a:ext cx="1515033" cy="484463"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4428,7 +4468,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100"/>
-            <a:t>Not ok</a:t>
+            <a:t>Not ok - is dat een optie?</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -4438,13 +4478,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>140075</xdr:colOff>
+      <xdr:colOff>151092</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>16435</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>566460</xdr:colOff>
+      <xdr:rowOff>53788</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>336179</xdr:colOff>
       <xdr:row>81</xdr:row>
       <xdr:rowOff>125136</xdr:rowOff>
     </xdr:to>
@@ -4464,8 +4504,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="7156916" y="13506358"/>
-          <a:ext cx="482231" cy="2264150"/>
+          <a:off x="7236290" y="13139178"/>
+          <a:ext cx="429937" cy="2587628"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -4566,13 +4606,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>566457</xdr:colOff>
+      <xdr:colOff>560481</xdr:colOff>
       <xdr:row>79</xdr:row>
-      <xdr:rowOff>16437</xdr:rowOff>
+      <xdr:rowOff>53790</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>140074</xdr:colOff>
+      <xdr:colOff>151091</xdr:colOff>
       <xdr:row>81</xdr:row>
       <xdr:rowOff>144187</xdr:rowOff>
     </xdr:to>
@@ -4592,8 +4632,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="5922214" y="14554856"/>
-          <a:ext cx="501280" cy="186205"/>
+          <a:off x="5837329" y="14346895"/>
+          <a:ext cx="448986" cy="191245"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst/>
@@ -4622,15 +4662,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>303680</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>63874</xdr:rowOff>
+      <xdr:colOff>339539</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>81804</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>252879</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>104589</xdr:rowOff>
+      <xdr:colOff>288738</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>122519</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4645,8 +4685,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5204386" y="15752109"/>
-          <a:ext cx="1786964" cy="1348068"/>
+          <a:off x="5144621" y="15321804"/>
+          <a:ext cx="1751105" cy="1295774"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4686,7 +4726,18 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t>application succeeded</a:t>
+            <a:t>application succeeded.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="nl-NL" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
+            <a:t>Vermeldt oa nieuw IBAN</a:t>
           </a:r>
           <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
@@ -4763,15 +4814,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>566457</xdr:colOff>
+      <xdr:colOff>560480</xdr:colOff>
       <xdr:row>83</xdr:row>
       <xdr:rowOff>48936</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>584574</xdr:colOff>
-      <xdr:row>86</xdr:row>
-      <xdr:rowOff>63874</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>13820</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>81804</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4788,12 +4839,14 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6079751" y="15176877"/>
-          <a:ext cx="18117" cy="575232"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="5797458" y="15099088"/>
+          <a:ext cx="391456" cy="53975"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
         </a:prstGeom>
         <a:ln>
           <a:tailEnd type="triangle"/>
@@ -4874,7 +4927,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="nl-NL" sz="1100" baseline="0"/>
-            <a:t> confirmation (check db for emailaddress)</a:t>
+            <a:t> confirmation </a:t>
           </a:r>
           <a:endParaRPr lang="nl-NL" sz="1100"/>
         </a:p>
@@ -4885,13 +4938,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>584574</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>104589</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>595780</xdr:colOff>
+      <xdr:colOff>589802</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>122519</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>13821</xdr:colOff>
       <xdr:row>95</xdr:row>
       <xdr:rowOff>166967</xdr:rowOff>
     </xdr:to>
@@ -4910,9 +4963,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6097868" y="17100177"/>
-          <a:ext cx="11206" cy="435908"/>
+        <a:xfrm flipH="1">
+          <a:off x="5995520" y="16617578"/>
+          <a:ext cx="24654" cy="582330"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -5366,13 +5419,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77628A9-8BFD-49FE-9150-0DF4141E1CF8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S100" sqref="S100"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>